<commit_message>
Updates in the climate ccs file
</commit_message>
<xml_diff>
--- a/models/14sectors_cat/climate.xlsx
+++ b/models/14sectors_cat/climate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\OneDrive\01.Feina_CREAF\07.Vensim_models\pymedeas2_vensim\models_for_pymedeas2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.Feina_CREAF\06.Git_Repos\pymedeas2_vensim\models_for_pymedeas2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97EF910-A928-4695-9AA9-0009ED2DDA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8C13EF-B14C-4379-8868-825F35A271F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11028" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13995" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -3406,7 +3406,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
@@ -3414,7 +3414,7 @@
     <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal 8" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3788,18 +3788,18 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="16" width="9.109375" customWidth="1"/>
-    <col min="19" max="19" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="16" width="9.140625" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" customWidth="1"/>
     <col min="20" max="20" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A1" s="194" t="s">
         <v>0</v>
       </c>
@@ -3850,7 +3850,7 @@
       <c r="AY1" s="2"/>
       <c r="AZ1" s="2"/>
     </row>
-    <row r="2" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -3905,7 +3905,7 @@
       <c r="AY2" s="2"/>
       <c r="AZ2" s="2"/>
     </row>
-    <row r="3" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
@@ -3929,7 +3929,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
@@ -4098,7 +4098,7 @@
       <c r="FH5" s="2"/>
       <c r="FI5" s="2"/>
     </row>
-    <row r="6" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
@@ -4267,7 +4267,7 @@
       <c r="FH6" s="2"/>
       <c r="FI6" s="2"/>
     </row>
-    <row r="7" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
@@ -4286,7 +4286,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>9</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>12400</v>
       </c>
     </row>
-    <row r="9" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="10" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>11</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>3170</v>
       </c>
     </row>
-    <row r="11" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="12" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>13</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>3350</v>
       </c>
     </row>
-    <row r="14" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>15</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="15" spans="1:165" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:165" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>16</v>
       </c>
@@ -4374,14 +4374,14 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="195" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="195"/>
       <c r="C17" s="195"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>18</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>0.16520000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>20</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>0.1033</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>21</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>22</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>23</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>7.7777777777777807E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>24</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>25</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>7.7777777777777807E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>26</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>28</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>0.106009479</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>29</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>6.9879147000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>30</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>4.9355450000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>31</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>8.9826223999999996E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>32</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>0.10030963699999999</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>33</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>8.5971564E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>34</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>36</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>37</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>38</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>39</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>40</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>41</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>42</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>43</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>44</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>45</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>46</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>47</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>48</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="196" t="s">
         <v>49</v>
       </c>
@@ -4760,14 +4760,14 @@
       <c r="C48" s="196"/>
       <c r="D48" s="196"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="17"/>
       <c r="B49" s="18"/>
       <c r="C49" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>51</v>
       </c>
@@ -4779,7 +4779,7 @@
       </c>
       <c r="G50" s="31"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>53</v>
       </c>
@@ -4791,7 +4791,7 @@
       </c>
       <c r="G51" s="32"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>54</v>
       </c>
@@ -4803,7 +4803,7 @@
       </c>
       <c r="G52" s="21"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="197" t="s">
         <v>55</v>
       </c>
@@ -4811,7 +4811,7 @@
       <c r="C54" s="197"/>
       <c r="D54" s="197"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="33"/>
       <c r="B55" s="33"/>
       <c r="C55" s="19" t="s">
@@ -4821,7 +4821,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>58</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>722.22799999999995</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>59</v>
       </c>
@@ -4873,27 +4873,27 @@
       <selection activeCell="AD202" activeCellId="1" sqref="A116:A117 AD202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5546875" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" customWidth="1"/>
-    <col min="9" max="9" width="25.5546875" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
     <col min="13" max="13" width="19" customWidth="1"/>
-    <col min="14" max="14" width="24.5546875" customWidth="1"/>
-    <col min="15" max="15" width="16.88671875" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" customWidth="1"/>
-    <col min="19" max="19" width="16.109375" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" customWidth="1"/>
     <col min="20" max="20" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="220" t="s">
         <v>60</v>
       </c>
@@ -4905,7 +4905,7 @@
       <c r="F1" s="220"/>
       <c r="G1" s="220"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>62</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>1076.17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>66</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>988.15800000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>69</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>10.465199999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>72</v>
       </c>
@@ -4981,7 +4981,7 @@
       <c r="F5" s="221"/>
       <c r="G5" s="43"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>75</v>
       </c>
@@ -5005,7 +5005,7 @@
       <c r="J6" s="45"/>
       <c r="K6" s="45"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
         <v>78</v>
       </c>
@@ -5029,7 +5029,7 @@
       <c r="J7" s="45"/>
       <c r="K7" s="45"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>80</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>10.2768</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>82</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>10.265000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>84</v>
       </c>
@@ -5085,7 +5085,7 @@
       <c r="F10" s="221"/>
       <c r="G10" s="50"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>86</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>0.35060000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>88</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>0.18140000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>89</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>0.1492</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>90</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>3.8000000000000002E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>92</v>
       </c>
@@ -5176,14 +5176,14 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="222" t="s">
         <v>94</v>
       </c>
       <c r="B16" s="222"/>
       <c r="C16" s="57"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
         <v>77</v>
       </c>
@@ -5199,7 +5199,7 @@
       <c r="F17" s="215"/>
       <c r="G17" s="215"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>79</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>5.35</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>81</v>
       </c>
@@ -5239,7 +5239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>83</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
         <v>101</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
         <v>103</v>
       </c>
@@ -5301,7 +5301,7 @@
       </c>
       <c r="H22" s="62"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
         <v>106</v>
       </c>
@@ -5321,7 +5321,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
         <v>108</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
         <v>109</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="70" t="s">
         <v>113</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>360.3</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="216" t="s">
         <v>116</v>
       </c>
@@ -5380,7 +5380,7 @@
       <c r="C29" s="216"/>
       <c r="D29" s="216"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="74" t="s">
         <v>117</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="76" t="s">
         <v>119</v>
       </c>
@@ -5406,7 +5406,7 @@
       </c>
       <c r="D31" s="217"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="76" t="s">
         <v>121</v>
       </c>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="D32" s="217"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="78" t="s">
         <v>123</v>
       </c>
@@ -5430,7 +5430,7 @@
       </c>
       <c r="D33" s="217"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="76" t="s">
         <v>124</v>
       </c>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="D34" s="217"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="76" t="s">
         <v>125</v>
       </c>
@@ -5454,7 +5454,7 @@
       </c>
       <c r="D35" s="217"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="76" t="s">
         <v>126</v>
       </c>
@@ -5466,7 +5466,7 @@
       </c>
       <c r="D36" s="217"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="76" t="s">
         <v>128</v>
       </c>
@@ -5478,7 +5478,7 @@
       </c>
       <c r="D37" s="217"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="81" t="s">
         <v>129</v>
       </c>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="D38" s="217"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="74" t="s">
         <v>130</v>
       </c>
@@ -5504,7 +5504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="76" t="s">
         <v>132</v>
       </c>
@@ -5516,7 +5516,7 @@
       </c>
       <c r="D40" s="218"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="81" t="s">
         <v>133</v>
       </c>
@@ -5528,7 +5528,7 @@
       </c>
       <c r="D41" s="218"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="74" t="s">
         <v>135</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="76" t="s">
         <v>138</v>
       </c>
@@ -5554,7 +5554,7 @@
       </c>
       <c r="D43" s="219"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="76" t="s">
         <v>139</v>
       </c>
@@ -5566,7 +5566,7 @@
       </c>
       <c r="D44" s="219"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="81" t="s">
         <v>140</v>
       </c>
@@ -5578,7 +5578,7 @@
       </c>
       <c r="D45" s="219"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="74" t="s">
         <v>142</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="76" t="s">
         <v>143</v>
       </c>
@@ -5604,7 +5604,7 @@
       </c>
       <c r="D47" s="211"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="76" t="s">
         <v>144</v>
       </c>
@@ -5616,7 +5616,7 @@
       </c>
       <c r="D48" s="211"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="88" t="s">
         <v>145</v>
       </c>
@@ -5628,7 +5628,7 @@
       </c>
       <c r="D49" s="211"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="91" t="s">
         <v>146</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="95" t="s">
         <v>150</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="96" t="s">
         <v>8</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="96" t="s">
         <v>9</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="96" t="s">
         <v>10</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="96" t="s">
         <v>11</v>
       </c>
@@ -5712,7 +5712,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="96" t="s">
         <v>12</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="96" t="s">
         <v>13</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="96" t="s">
         <v>14</v>
       </c>
@@ -5754,7 +5754,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="96" t="s">
         <v>15</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="97" t="s">
         <v>16</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="100" t="s">
         <v>151</v>
       </c>
@@ -5793,14 +5793,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="212" t="s">
         <v>152</v>
       </c>
       <c r="B64" s="212"/>
       <c r="C64" s="212"/>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="76" t="s">
         <v>153</v>
       </c>
@@ -5811,14 +5811,14 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="102" t="s">
         <v>155</v>
       </c>
       <c r="B66" s="103"/>
       <c r="C66" s="57"/>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="76" t="s">
         <v>156</v>
       </c>
@@ -5829,7 +5829,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="76" t="s">
         <v>157</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="76" t="s">
         <v>159</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="76" t="s">
         <v>161</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" s="76" t="s">
         <v>162</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72" s="76" t="s">
         <v>163</v>
       </c>
@@ -5884,7 +5884,7 @@
         <v>2.0100000000000001E-5</v>
       </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" s="76" t="s">
         <v>164</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>5.3099999999999999E-15</v>
       </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" s="76" t="s">
         <v>165</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" s="76" t="s">
         <v>166</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" s="81" t="s">
         <v>167</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78" s="107" t="s">
         <v>63</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" s="58" t="s">
         <v>168</v>
       </c>
@@ -6146,7 +6146,7 @@
         <v>0.10374</v>
       </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" s="111"/>
       <c r="B80" s="2"/>
       <c r="C80" s="112"/>
@@ -6179,7 +6179,7 @@
       <c r="AD80" s="12"/>
       <c r="AE80" s="12"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="107" t="s">
         <v>63</v>
       </c>
@@ -6197,7 +6197,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="58" t="s">
         <v>169</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>-0.89600000000000002</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="107" t="s">
         <v>63</v>
       </c>
@@ -6253,7 +6253,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="58" t="s">
         <v>170</v>
       </c>
@@ -6291,7 +6291,7 @@
         <v>-0.32284000000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="58" t="s">
         <v>171</v>
       </c>
@@ -6327,7 +6327,7 @@
         <v>-0.22386</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="58" t="s">
         <v>172</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>-0.32754</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="58" t="s">
         <v>173</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>-8.8349999999999998E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="100" t="s">
         <v>174</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="100" t="s">
         <v>175</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="119" t="s">
         <v>176</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="214" t="s">
         <v>177</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>130.44239999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="214"/>
       <c r="B96" s="207"/>
       <c r="C96" s="19" t="s">
@@ -6563,7 +6563,7 @@
         <v>207.98699999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="214"/>
       <c r="B97" s="207"/>
       <c r="C97" s="19" t="s">
@@ -6609,7 +6609,7 @@
         <v>210.3058</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="214"/>
       <c r="B98" s="207"/>
       <c r="C98" s="130" t="s">
@@ -6655,7 +6655,7 @@
         <v>558.01499999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="206" t="s">
         <v>182</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>5.2823018181818204</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="206"/>
       <c r="B100" s="207"/>
       <c r="C100" s="19" t="s">
@@ -6757,7 +6757,7 @@
         <v>8.1117018181818192</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="206"/>
       <c r="B101" s="207"/>
       <c r="C101" s="19" t="s">
@@ -6806,7 +6806,7 @@
         <v>12.2700009090909</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="206"/>
       <c r="B102" s="207"/>
       <c r="C102" s="130" t="s">
@@ -6855,7 +6855,7 @@
         <v>15.775600909090899</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="208" t="s">
         <v>184</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>109.21</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="208"/>
       <c r="B104" s="209"/>
       <c r="C104" s="19" t="s">
@@ -6951,7 +6951,7 @@
         <v>11396.4</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="208"/>
       <c r="B105" s="209"/>
       <c r="C105" s="19" t="s">
@@ -6997,7 +6997,7 @@
         <v>20799</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="208"/>
       <c r="B106" s="209"/>
       <c r="C106" s="151" t="s">
@@ -7043,7 +7043,7 @@
         <v>10765.4</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="206" t="s">
         <v>186</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>44.2</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="206"/>
       <c r="B108" s="210"/>
       <c r="C108" s="156" t="s">
@@ -7139,7 +7139,7 @@
         <v>6434.3</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="206"/>
       <c r="B109" s="210"/>
       <c r="C109" s="156" t="s">
@@ -7185,7 +7185,7 @@
         <v>9497.1</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="206"/>
       <c r="B110" s="210"/>
       <c r="C110" s="157" t="s">
@@ -7231,7 +7231,7 @@
         <v>16922.3</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="160" t="s">
         <v>187</v>
       </c>
@@ -7251,7 +7251,7 @@
       <c r="O111" s="161"/>
       <c r="P111" s="162"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="201" t="s">
         <v>8</v>
       </c>
@@ -7301,7 +7301,7 @@
         <v>235392</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="201"/>
       <c r="B113" s="202"/>
       <c r="C113" s="19" t="s">
@@ -7347,7 +7347,7 @@
         <v>409075</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="201"/>
       <c r="B114" s="202"/>
       <c r="C114" s="19" t="s">
@@ -7393,7 +7393,7 @@
         <v>170500</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="201"/>
       <c r="B115" s="202"/>
       <c r="C115" s="19" t="s">
@@ -7439,7 +7439,7 @@
         <v>703459</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="201" t="s">
         <v>9</v>
       </c>
@@ -7489,7 +7489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="201"/>
       <c r="B117" s="202"/>
       <c r="C117" s="19" t="s">
@@ -7535,7 +7535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="201"/>
       <c r="B118" s="202"/>
       <c r="C118" s="19" t="s">
@@ -7581,7 +7581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="201"/>
       <c r="B119" s="202"/>
       <c r="C119" s="19" t="s">
@@ -7627,7 +7627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="201" t="s">
         <v>10</v>
       </c>
@@ -7677,7 +7677,7 @@
         <v>81227</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="201"/>
       <c r="B121" s="202"/>
       <c r="C121" s="19" t="s">
@@ -7723,7 +7723,7 @@
         <v>81227</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="201"/>
       <c r="B122" s="202"/>
       <c r="C122" s="19" t="s">
@@ -7769,7 +7769,7 @@
         <v>81227</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="201"/>
       <c r="B123" s="202"/>
       <c r="C123" s="19" t="s">
@@ -7815,7 +7815,7 @@
         <v>81227</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="201" t="s">
         <v>11</v>
       </c>
@@ -7865,7 +7865,7 @@
         <v>148214</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="201"/>
       <c r="B125" s="202"/>
       <c r="C125" s="19" t="s">
@@ -7911,7 +7911,7 @@
         <v>23006</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="201"/>
       <c r="B126" s="202"/>
       <c r="C126" s="19" t="s">
@@ -7957,7 +7957,7 @@
         <v>11699</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="201"/>
       <c r="B127" s="202"/>
       <c r="C127" s="19" t="s">
@@ -8003,7 +8003,7 @@
         <v>148304</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="201" t="s">
         <v>12</v>
       </c>
@@ -8053,7 +8053,7 @@
         <v>77457</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" s="201"/>
       <c r="B129" s="202"/>
       <c r="C129" s="19" t="s">
@@ -8099,7 +8099,7 @@
         <v>46270</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" s="201"/>
       <c r="B130" s="202"/>
       <c r="C130" s="19" t="s">
@@ -8145,7 +8145,7 @@
         <v>9099</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" s="201"/>
       <c r="B131" s="202"/>
       <c r="C131" s="19" t="s">
@@ -8191,7 +8191,7 @@
         <v>46842</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" s="201" t="s">
         <v>13</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" s="201"/>
       <c r="B133" s="202"/>
       <c r="C133" s="19" t="s">
@@ -8287,7 +8287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" s="201"/>
       <c r="B134" s="202"/>
       <c r="C134" s="19" t="s">
@@ -8333,7 +8333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" s="201"/>
       <c r="B135" s="202"/>
       <c r="C135" s="19" t="s">
@@ -8379,7 +8379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" s="201" t="s">
         <v>14</v>
       </c>
@@ -8429,7 +8429,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" s="201"/>
       <c r="B137" s="202"/>
       <c r="C137" s="19" t="s">
@@ -8475,7 +8475,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" s="201"/>
       <c r="B138" s="202"/>
       <c r="C138" s="19" t="s">
@@ -8521,7 +8521,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" s="201"/>
       <c r="B139" s="202"/>
       <c r="C139" s="19" t="s">
@@ -8567,7 +8567,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" s="203" t="s">
         <v>15</v>
       </c>
@@ -8617,7 +8617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" s="203"/>
       <c r="B141" s="202"/>
       <c r="C141" s="19" t="s">
@@ -8663,7 +8663,7 @@
         <v>82888</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" s="203"/>
       <c r="B142" s="202"/>
       <c r="C142" s="19" t="s">
@@ -8709,7 +8709,7 @@
         <v>65062</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" s="203"/>
       <c r="B143" s="202"/>
       <c r="C143" s="19" t="s">
@@ -8755,7 +8755,7 @@
         <v>131805</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" s="204" t="s">
         <v>16</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" s="204"/>
       <c r="B145" s="205"/>
       <c r="C145" s="19" t="s">
@@ -8851,7 +8851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" s="204"/>
       <c r="B146" s="205"/>
       <c r="C146" s="19" t="s">
@@ -8897,7 +8897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" s="204"/>
       <c r="B147" s="205"/>
       <c r="C147" s="130" t="s">
@@ -8943,10 +8943,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C149" s="176"/>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" s="177" t="s">
         <v>188</v>
       </c>
@@ -8990,7 +8990,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" s="200" t="s">
         <v>189</v>
       </c>
@@ -9034,7 +9034,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" s="200"/>
       <c r="B153" s="17" t="s">
         <v>53</v>
@@ -9076,7 +9076,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" s="200"/>
       <c r="B154" s="17" t="s">
         <v>54</v>
@@ -9118,7 +9118,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" s="199" t="s">
         <v>190</v>
       </c>
@@ -9162,7 +9162,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" s="199"/>
       <c r="B156" s="17" t="s">
         <v>53</v>
@@ -9204,7 +9204,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" s="199"/>
       <c r="B157" s="17" t="s">
         <v>54</v>
@@ -9246,7 +9246,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" s="199" t="s">
         <v>191</v>
       </c>
@@ -9302,7 +9302,7 @@
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" s="199"/>
       <c r="B159" s="17" t="s">
         <v>53</v>
@@ -9344,7 +9344,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" s="199"/>
       <c r="B160" s="17" t="s">
         <v>54</v>
@@ -9386,7 +9386,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" s="199" t="s">
         <v>192</v>
       </c>
@@ -9430,7 +9430,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" s="199"/>
       <c r="B162" s="17" t="s">
         <v>53</v>
@@ -9472,7 +9472,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" s="199"/>
       <c r="B163" s="17" t="s">
         <v>54</v>
@@ -9514,7 +9514,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" s="199" t="s">
         <v>193</v>
       </c>
@@ -9558,7 +9558,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" s="199"/>
       <c r="B165" s="17" t="s">
         <v>53</v>
@@ -9600,7 +9600,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" s="199"/>
       <c r="B166" s="17" t="s">
         <v>54</v>
@@ -9642,7 +9642,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" s="199" t="s">
         <v>194</v>
       </c>
@@ -9686,7 +9686,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A168" s="199"/>
       <c r="B168" s="17" t="s">
         <v>53</v>
@@ -9728,7 +9728,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169" s="199"/>
       <c r="B169" s="17" t="s">
         <v>54</v>
@@ -9770,7 +9770,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A170" s="199" t="s">
         <v>195</v>
       </c>
@@ -9814,7 +9814,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171" s="199"/>
       <c r="B171" s="17" t="s">
         <v>53</v>
@@ -9856,7 +9856,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" s="199"/>
       <c r="B172" s="17" t="s">
         <v>54</v>
@@ -9898,7 +9898,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" s="199" t="s">
         <v>196</v>
       </c>
@@ -9942,7 +9942,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" s="199"/>
       <c r="B174" s="17" t="s">
         <v>53</v>
@@ -9984,7 +9984,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" s="199"/>
       <c r="B175" s="17" t="s">
         <v>54</v>
@@ -10026,7 +10026,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" s="199" t="s">
         <v>197</v>
       </c>
@@ -10070,7 +10070,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A177" s="199"/>
       <c r="B177" s="17" t="s">
         <v>53</v>
@@ -10112,7 +10112,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178" s="199"/>
       <c r="B178" s="17" t="s">
         <v>54</v>
@@ -10154,7 +10154,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A179" s="199" t="s">
         <v>198</v>
       </c>
@@ -10198,7 +10198,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180" s="199"/>
       <c r="B180" s="17" t="s">
         <v>53</v>
@@ -10240,7 +10240,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A181" s="199"/>
       <c r="B181" s="17" t="s">
         <v>54</v>
@@ -10282,7 +10282,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" s="199" t="s">
         <v>199</v>
       </c>
@@ -10326,7 +10326,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183" s="199"/>
       <c r="B183" s="17" t="s">
         <v>53</v>
@@ -10368,7 +10368,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184" s="199"/>
       <c r="B184" s="17" t="s">
         <v>54</v>
@@ -10410,7 +10410,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185" s="199" t="s">
         <v>200</v>
       </c>
@@ -10454,7 +10454,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A186" s="199"/>
       <c r="B186" s="17" t="s">
         <v>53</v>
@@ -10496,7 +10496,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A187" s="199"/>
       <c r="B187" s="17" t="s">
         <v>54</v>
@@ -10538,7 +10538,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A188" s="199" t="s">
         <v>201</v>
       </c>
@@ -10582,7 +10582,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A189" s="199"/>
       <c r="B189" s="17" t="s">
         <v>53</v>
@@ -10624,7 +10624,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A190" s="199"/>
       <c r="B190" s="17" t="s">
         <v>54</v>
@@ -10666,7 +10666,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A191" s="199" t="s">
         <v>202</v>
       </c>
@@ -10710,7 +10710,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A192" s="199"/>
       <c r="B192" s="17" t="s">
         <v>53</v>
@@ -10752,7 +10752,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="193" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A193" s="199"/>
       <c r="B193" s="17" t="s">
         <v>54</v>
@@ -10794,7 +10794,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="194" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A194" s="199" t="s">
         <v>203</v>
       </c>
@@ -10838,7 +10838,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="195" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A195" s="199"/>
       <c r="B195" s="17" t="s">
         <v>53</v>
@@ -10880,7 +10880,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="196" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A196" s="199"/>
       <c r="B196" s="17" t="s">
         <v>54</v>
@@ -10922,7 +10922,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="197" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A197" s="177" t="s">
         <v>204</v>
       </c>
@@ -10966,7 +10966,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="198" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A198" s="198" t="s">
         <v>205</v>
       </c>
@@ -11010,7 +11010,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="199" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A199" s="198"/>
       <c r="B199" s="17" t="s">
         <v>207</v>
@@ -11052,7 +11052,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="201" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A201" s="197" t="s">
         <v>208</v>
       </c>
@@ -11086,7 +11086,7 @@
       <c r="AC201" s="197"/>
       <c r="AD201" s="197"/>
     </row>
-    <row r="202" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A202" s="17" t="s">
         <v>209</v>
       </c>
@@ -11178,7 +11178,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="203" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A203" s="17" t="s">
         <v>210</v>
       </c>
@@ -11343,21 +11343,21 @@
   </sheetPr>
   <dimension ref="A1:AD110"/>
   <sheetViews>
-    <sheetView topLeftCell="Q97" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109:AD109"/>
+    <sheetView topLeftCell="A61" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="16" width="9.109375" customWidth="1"/>
-    <col min="19" max="19" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="16" width="9.140625" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" customWidth="1"/>
     <col min="20" max="20" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="119" t="s">
         <v>176</v>
       </c>
@@ -11403,7 +11403,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="214" t="s">
         <v>177</v>
       </c>
@@ -11453,7 +11453,7 @@
         <v>11.921069910256</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="214"/>
       <c r="B3" s="207"/>
       <c r="C3" s="19" t="s">
@@ -11499,7 +11499,7 @@
         <v>22.886043946264</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="214"/>
       <c r="B4" s="207"/>
       <c r="C4" s="19" t="s">
@@ -11545,7 +11545,7 @@
         <v>20.342332826886199</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="214"/>
       <c r="B5" s="207"/>
       <c r="C5" s="130" t="s">
@@ -11591,7 +11591,7 @@
         <v>68.009924943051004</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="206" t="s">
         <v>182</v>
       </c>
@@ -11641,7 +11641,7 @@
         <v>0.73661068486611003</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="206"/>
       <c r="B7" s="207"/>
       <c r="C7" s="19" t="s">
@@ -11687,7 +11687,7 @@
         <v>1.1268261051364801</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="206"/>
       <c r="B8" s="207"/>
       <c r="C8" s="19" t="s">
@@ -11733,7 +11733,7 @@
         <v>1.6384187068570799</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="206"/>
       <c r="B9" s="207"/>
       <c r="C9" s="130" t="s">
@@ -11779,7 +11779,7 @@
         <v>2.11497123965471</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="208" t="s">
         <v>184</v>
       </c>
@@ -11829,7 +11829,7 @@
         <v>84.195230848646204</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="208"/>
       <c r="B11" s="209"/>
       <c r="C11" s="19" t="s">
@@ -11875,7 +11875,7 @@
         <v>1235.39958147164</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="208"/>
       <c r="B12" s="209"/>
       <c r="C12" s="19" t="s">
@@ -11921,7 +11921,7 @@
         <v>1076.9551142068599</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="208"/>
       <c r="B13" s="209"/>
       <c r="C13" s="151" t="s">
@@ -11967,7 +11967,7 @@
         <v>1164.1662905288499</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="206" t="s">
         <v>186</v>
       </c>
@@ -12017,7 +12017,7 @@
         <v>3.6037505095801099</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="206"/>
       <c r="B15" s="210"/>
       <c r="C15" s="156" t="s">
@@ -12063,7 +12063,7 @@
         <v>614.372458181561</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="206"/>
       <c r="B16" s="210"/>
       <c r="C16" s="156" t="s">
@@ -12109,7 +12109,7 @@
         <v>660.00463302575201</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="206"/>
       <c r="B17" s="210"/>
       <c r="C17" s="157" t="s">
@@ -12155,7 +12155,7 @@
         <v>1297.22499041778</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="160" t="s">
         <v>187</v>
       </c>
@@ -12175,7 +12175,7 @@
       <c r="O18" s="161"/>
       <c r="P18" s="162"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="201" t="s">
         <v>8</v>
       </c>
@@ -12225,7 +12225,7 @@
         <v>57163.609355399502</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="201"/>
       <c r="B20" s="202"/>
       <c r="C20" s="19" t="s">
@@ -12271,7 +12271,7 @@
         <v>109302.76726849801</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="201"/>
       <c r="B21" s="202"/>
       <c r="C21" s="19" t="s">
@@ -12317,7 +12317,7 @@
         <v>44445.072145781698</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="201"/>
       <c r="B22" s="202"/>
       <c r="C22" s="19" t="s">
@@ -12363,7 +12363,7 @@
         <v>175905.10896120299</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="201" t="s">
         <v>9</v>
       </c>
@@ -12413,7 +12413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="201"/>
       <c r="B24" s="202"/>
       <c r="C24" s="19" t="s">
@@ -12459,7 +12459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="201"/>
       <c r="B25" s="202"/>
       <c r="C25" s="19" t="s">
@@ -12505,7 +12505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="201"/>
       <c r="B26" s="202"/>
       <c r="C26" s="19" t="s">
@@ -12551,7 +12551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="201" t="s">
         <v>10</v>
       </c>
@@ -12601,7 +12601,7 @@
         <v>2545.0486347098399</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="201"/>
       <c r="B28" s="202"/>
       <c r="C28" s="19" t="s">
@@ -12647,7 +12647,7 @@
         <v>2545.0486347098399</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="201"/>
       <c r="B29" s="202"/>
       <c r="C29" s="19" t="s">
@@ -12693,7 +12693,7 @@
         <v>2545.0486347098399</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="201"/>
       <c r="B30" s="202"/>
       <c r="C30" s="19" t="s">
@@ -12739,7 +12739,7 @@
         <v>2545.0486347098399</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="201" t="s">
         <v>11</v>
       </c>
@@ -12789,7 +12789,7 @@
         <v>42731.323655643901</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="201"/>
       <c r="B32" s="202"/>
       <c r="C32" s="19" t="s">
@@ -12835,7 +12835,7 @@
         <v>10177.1405025204</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="201"/>
       <c r="B33" s="202"/>
       <c r="C33" s="19" t="s">
@@ -12881,7 +12881,7 @@
         <v>10914.5336222961</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="201"/>
       <c r="B34" s="202"/>
       <c r="C34" s="19" t="s">
@@ -12927,7 +12927,7 @@
         <v>32476.395605140999</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="201" t="s">
         <v>12</v>
       </c>
@@ -12977,7 +12977,7 @@
         <v>27985.366510455198</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="201"/>
       <c r="B36" s="202"/>
       <c r="C36" s="19" t="s">
@@ -13023,7 +13023,7 @@
         <v>25514.666894960999</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="201"/>
       <c r="B37" s="202"/>
       <c r="C37" s="19" t="s">
@@ -13069,7 +13069,7 @@
         <v>15742.6474147098</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="201"/>
       <c r="B38" s="202"/>
       <c r="C38" s="19" t="s">
@@ -13115,7 +13115,7 @@
         <v>13785.713981987399</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="201" t="s">
         <v>13</v>
       </c>
@@ -13165,7 +13165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="201"/>
       <c r="B40" s="202"/>
       <c r="C40" s="19" t="s">
@@ -13211,7 +13211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="201"/>
       <c r="B41" s="202"/>
       <c r="C41" s="19" t="s">
@@ -13257,7 +13257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="201"/>
       <c r="B42" s="202"/>
       <c r="C42" s="19" t="s">
@@ -13303,7 +13303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="201" t="s">
         <v>14</v>
       </c>
@@ -13353,7 +13353,7 @@
         <v>18.1522990681962</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="201"/>
       <c r="B44" s="202"/>
       <c r="C44" s="19" t="s">
@@ -13399,7 +13399,7 @@
         <v>4.03659154324962</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="201"/>
       <c r="B45" s="202"/>
       <c r="C45" s="19" t="s">
@@ -13445,7 +13445,7 @@
         <v>5.4829387755101999</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="201"/>
       <c r="B46" s="202"/>
       <c r="C46" s="19" t="s">
@@ -13491,7 +13491,7 @@
         <v>14.1226491060856</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="203" t="s">
         <v>15</v>
       </c>
@@ -13541,7 +13541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="203"/>
       <c r="B48" s="202"/>
       <c r="C48" s="19" t="s">
@@ -13587,7 +13587,7 @@
         <v>1901.1512525036401</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="203"/>
       <c r="B49" s="202"/>
       <c r="C49" s="19" t="s">
@@ -13633,7 +13633,7 @@
         <v>1146.89297285614</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="203"/>
       <c r="B50" s="202"/>
       <c r="C50" s="19" t="s">
@@ -13679,7 +13679,7 @@
         <v>1716.1620203259199</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="204" t="s">
         <v>16</v>
       </c>
@@ -13729,7 +13729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="204"/>
       <c r="B52" s="205"/>
       <c r="C52" s="19" t="s">
@@ -13775,7 +13775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="204"/>
       <c r="B53" s="205"/>
       <c r="C53" s="19" t="s">
@@ -13821,7 +13821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="204"/>
       <c r="B54" s="205"/>
       <c r="C54" s="130" t="s">
@@ -13867,7 +13867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="177" t="s">
         <v>188</v>
       </c>
@@ -13911,7 +13911,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="200" t="s">
         <v>189</v>
       </c>
@@ -13955,7 +13955,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="200"/>
       <c r="B60" s="17" t="s">
         <v>53</v>
@@ -13997,7 +13997,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="200"/>
       <c r="B61" s="17" t="s">
         <v>54</v>
@@ -14039,7 +14039,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="200" t="s">
         <v>190</v>
       </c>
@@ -14083,7 +14083,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="200"/>
       <c r="B63" s="17" t="s">
         <v>53</v>
@@ -14125,7 +14125,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="200"/>
       <c r="B64" s="17" t="s">
         <v>54</v>
@@ -14167,7 +14167,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="200" t="s">
         <v>191</v>
       </c>
@@ -14223,7 +14223,7 @@
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="200"/>
       <c r="B66" s="17" t="s">
         <v>53</v>
@@ -14265,7 +14265,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="200"/>
       <c r="B67" s="17" t="s">
         <v>54</v>
@@ -14307,7 +14307,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="200" t="s">
         <v>192</v>
       </c>
@@ -14351,7 +14351,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="200"/>
       <c r="B69" s="17" t="s">
         <v>53</v>
@@ -14393,7 +14393,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="200"/>
       <c r="B70" s="17" t="s">
         <v>54</v>
@@ -14435,7 +14435,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="200" t="s">
         <v>193</v>
       </c>
@@ -14479,7 +14479,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="200"/>
       <c r="B72" s="17" t="s">
         <v>53</v>
@@ -14521,7 +14521,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="200"/>
       <c r="B73" s="17" t="s">
         <v>54</v>
@@ -14563,7 +14563,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="200" t="s">
         <v>194</v>
       </c>
@@ -14607,7 +14607,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="200"/>
       <c r="B75" s="17" t="s">
         <v>53</v>
@@ -14649,7 +14649,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="200"/>
       <c r="B76" s="17" t="s">
         <v>54</v>
@@ -14691,7 +14691,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="200" t="s">
         <v>195</v>
       </c>
@@ -14735,7 +14735,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="200"/>
       <c r="B78" s="17" t="s">
         <v>53</v>
@@ -14777,7 +14777,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="200"/>
       <c r="B79" s="17" t="s">
         <v>54</v>
@@ -14819,7 +14819,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="200" t="s">
         <v>196</v>
       </c>
@@ -14863,7 +14863,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="200"/>
       <c r="B81" s="17" t="s">
         <v>53</v>
@@ -14905,7 +14905,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="200"/>
       <c r="B82" s="17" t="s">
         <v>54</v>
@@ -14947,7 +14947,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="200" t="s">
         <v>197</v>
       </c>
@@ -14991,7 +14991,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="200"/>
       <c r="B84" s="17" t="s">
         <v>53</v>
@@ -15033,7 +15033,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="200"/>
       <c r="B85" s="17" t="s">
         <v>54</v>
@@ -15075,7 +15075,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="200" t="s">
         <v>198</v>
       </c>
@@ -15119,7 +15119,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="200"/>
       <c r="B87" s="17" t="s">
         <v>53</v>
@@ -15161,7 +15161,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="200"/>
       <c r="B88" s="17" t="s">
         <v>54</v>
@@ -15203,7 +15203,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="200" t="s">
         <v>199</v>
       </c>
@@ -15247,7 +15247,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="200"/>
       <c r="B90" s="17" t="s">
         <v>53</v>
@@ -15289,7 +15289,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="200"/>
       <c r="B91" s="17" t="s">
         <v>54</v>
@@ -15331,7 +15331,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="200" t="s">
         <v>200</v>
       </c>
@@ -15375,7 +15375,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="200"/>
       <c r="B93" s="17" t="s">
         <v>53</v>
@@ -15417,7 +15417,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="200"/>
       <c r="B94" s="17" t="s">
         <v>54</v>
@@ -15459,7 +15459,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="200" t="s">
         <v>201</v>
       </c>
@@ -15503,7 +15503,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="200"/>
       <c r="B96" s="17" t="s">
         <v>53</v>
@@ -15545,7 +15545,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="97" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A97" s="200"/>
       <c r="B97" s="17" t="s">
         <v>54</v>
@@ -15587,7 +15587,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="98" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A98" s="200" t="s">
         <v>202</v>
       </c>
@@ -15631,7 +15631,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="99" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A99" s="200"/>
       <c r="B99" s="17" t="s">
         <v>53</v>
@@ -15673,7 +15673,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="100" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A100" s="200"/>
       <c r="B100" s="17" t="s">
         <v>54</v>
@@ -15715,7 +15715,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="101" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A101" s="200" t="s">
         <v>203</v>
       </c>
@@ -15759,7 +15759,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="102" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A102" s="200"/>
       <c r="B102" s="17" t="s">
         <v>53</v>
@@ -15801,7 +15801,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="103" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A103" s="200"/>
       <c r="B103" s="17" t="s">
         <v>54</v>
@@ -15843,7 +15843,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="104" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A104" s="177" t="s">
         <v>204</v>
       </c>
@@ -15887,7 +15887,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="105" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A105" s="198" t="s">
         <v>205</v>
       </c>
@@ -15931,7 +15931,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="106" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A106" s="198"/>
       <c r="B106" s="17" t="s">
         <v>207</v>
@@ -15973,7 +15973,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="108" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A108" s="197" t="s">
         <v>208</v>
       </c>
@@ -16007,7 +16007,7 @@
       <c r="AC108" s="197"/>
       <c r="AD108" s="197"/>
     </row>
-    <row r="109" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A109" s="17" t="s">
         <v>209</v>
       </c>
@@ -16099,7 +16099,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="110" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A110" s="17" t="s">
         <v>210</v>
       </c>
@@ -16250,21 +16250,21 @@
   </sheetPr>
   <dimension ref="A1:AD118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U114" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AC117" sqref="C117:AC117"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80:N82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" customWidth="1"/>
-    <col min="4" max="16" width="9.109375" customWidth="1"/>
-    <col min="19" max="19" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="16" width="9.140625" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" customWidth="1"/>
     <col min="20" max="20" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="119" t="s">
         <v>176</v>
       </c>
@@ -16310,7 +16310,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="214" t="s">
         <v>177</v>
       </c>
@@ -16360,7 +16360,7 @@
         <v>2.3580512235E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="214"/>
       <c r="B3" s="207"/>
       <c r="C3" s="19" t="s">
@@ -16406,7 +16406,7 @@
         <v>0.94220365344000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="214"/>
       <c r="B4" s="207"/>
       <c r="C4" s="19" t="s">
@@ -16452,7 +16452,7 @@
         <v>1.1065580214399999</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="214"/>
       <c r="B5" s="207"/>
       <c r="C5" s="130" t="s">
@@ -16498,7 +16498,7 @@
         <v>3.6176096817040002</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="206" t="s">
         <v>182</v>
       </c>
@@ -16548,7 +16548,7 @@
         <v>1.03862106566122E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="206"/>
       <c r="B7" s="207"/>
       <c r="C7" s="19" t="s">
@@ -16594,7 +16594,7 @@
         <v>1.5888248082424401E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="206"/>
       <c r="B8" s="207"/>
       <c r="C8" s="19" t="s">
@@ -16640,7 +16640,7 @@
         <v>2.31017037666848E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="206"/>
       <c r="B9" s="207"/>
       <c r="C9" s="130" t="s">
@@ -16686,7 +16686,7 @@
         <v>2.9821094479131401E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="208" t="s">
         <v>184</v>
       </c>
@@ -16736,7 +16736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="208"/>
       <c r="B11" s="209"/>
       <c r="C11" s="19" t="s">
@@ -16782,7 +16782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="208"/>
       <c r="B12" s="209"/>
       <c r="C12" s="19" t="s">
@@ -16828,7 +16828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="208"/>
       <c r="B13" s="209"/>
       <c r="C13" s="151" t="s">
@@ -16874,7 +16874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="206" t="s">
         <v>186</v>
       </c>
@@ -16925,7 +16925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="206"/>
       <c r="B15" s="210"/>
       <c r="C15" s="156" t="s">
@@ -16972,7 +16972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="206"/>
       <c r="B16" s="210"/>
       <c r="C16" s="156" t="s">
@@ -17019,7 +17019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="206"/>
       <c r="B17" s="210"/>
       <c r="C17" s="157" t="s">
@@ -17066,7 +17066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="160" t="s">
         <v>187</v>
       </c>
@@ -17086,7 +17086,7 @@
       <c r="O18" s="161"/>
       <c r="P18" s="162"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="201" t="s">
         <v>8</v>
       </c>
@@ -17136,7 +17136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="201"/>
       <c r="B20" s="202"/>
       <c r="C20" s="19" t="s">
@@ -17182,7 +17182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="201"/>
       <c r="B21" s="202"/>
       <c r="C21" s="19" t="s">
@@ -17228,7 +17228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="201"/>
       <c r="B22" s="202"/>
       <c r="C22" s="19" t="s">
@@ -17274,7 +17274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="201" t="s">
         <v>9</v>
       </c>
@@ -17324,7 +17324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="201"/>
       <c r="B24" s="202"/>
       <c r="C24" s="19" t="s">
@@ -17370,7 +17370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="201"/>
       <c r="B25" s="202"/>
       <c r="C25" s="19" t="s">
@@ -17416,7 +17416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="201"/>
       <c r="B26" s="202"/>
       <c r="C26" s="19" t="s">
@@ -17462,7 +17462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="201" t="s">
         <v>10</v>
       </c>
@@ -17512,7 +17512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="201"/>
       <c r="B28" s="202"/>
       <c r="C28" s="19" t="s">
@@ -17558,7 +17558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="201"/>
       <c r="B29" s="202"/>
       <c r="C29" s="19" t="s">
@@ -17604,7 +17604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="201"/>
       <c r="B30" s="202"/>
       <c r="C30" s="19" t="s">
@@ -17650,7 +17650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="201" t="s">
         <v>11</v>
       </c>
@@ -17700,7 +17700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="201"/>
       <c r="B32" s="202"/>
       <c r="C32" s="19" t="s">
@@ -17746,7 +17746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="201"/>
       <c r="B33" s="202"/>
       <c r="C33" s="19" t="s">
@@ -17792,7 +17792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="201"/>
       <c r="B34" s="202"/>
       <c r="C34" s="19" t="s">
@@ -17838,7 +17838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="201" t="s">
         <v>12</v>
       </c>
@@ -17888,7 +17888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="201"/>
       <c r="B36" s="202"/>
       <c r="C36" s="19" t="s">
@@ -17934,7 +17934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="201"/>
       <c r="B37" s="202"/>
       <c r="C37" s="19" t="s">
@@ -17980,7 +17980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="201"/>
       <c r="B38" s="202"/>
       <c r="C38" s="19" t="s">
@@ -18026,7 +18026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="201" t="s">
         <v>13</v>
       </c>
@@ -18076,7 +18076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="201"/>
       <c r="B40" s="202"/>
       <c r="C40" s="19" t="s">
@@ -18122,7 +18122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="201"/>
       <c r="B41" s="202"/>
       <c r="C41" s="19" t="s">
@@ -18168,7 +18168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="201"/>
       <c r="B42" s="202"/>
       <c r="C42" s="19" t="s">
@@ -18214,7 +18214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="201" t="s">
         <v>14</v>
       </c>
@@ -18264,7 +18264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="201"/>
       <c r="B44" s="202"/>
       <c r="C44" s="19" t="s">
@@ -18310,7 +18310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="201"/>
       <c r="B45" s="202"/>
       <c r="C45" s="19" t="s">
@@ -18356,7 +18356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="201"/>
       <c r="B46" s="202"/>
       <c r="C46" s="19" t="s">
@@ -18402,7 +18402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="203" t="s">
         <v>15</v>
       </c>
@@ -18452,7 +18452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="203"/>
       <c r="B48" s="202"/>
       <c r="C48" s="19" t="s">
@@ -18498,7 +18498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="203"/>
       <c r="B49" s="202"/>
       <c r="C49" s="19" t="s">
@@ -18544,7 +18544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="203"/>
       <c r="B50" s="202"/>
       <c r="C50" s="19" t="s">
@@ -18590,7 +18590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="204" t="s">
         <v>16</v>
       </c>
@@ -18640,7 +18640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="204"/>
       <c r="B52" s="205"/>
       <c r="C52" s="19" t="s">
@@ -18686,7 +18686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="204"/>
       <c r="B53" s="205"/>
       <c r="C53" s="19" t="s">
@@ -18732,7 +18732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="204"/>
       <c r="B54" s="205"/>
       <c r="C54" s="130" t="s">
@@ -18778,7 +18778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="223" t="s">
         <v>212</v>
       </c>
@@ -18847,7 +18847,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="192" t="s">
         <v>213</v>
       </c>
@@ -18918,7 +18918,7 @@
         <v>3.3208666217348699E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="192" t="s">
         <v>215</v>
       </c>
@@ -18989,7 +18989,7 @@
         <v>4.2011336128108201E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="192" t="s">
         <v>217</v>
       </c>
@@ -19060,7 +19060,7 @@
         <v>4.2011336128108201E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="177" t="s">
         <v>188</v>
       </c>
@@ -19104,7 +19104,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="200" t="s">
         <v>189</v>
       </c>
@@ -19148,7 +19148,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="200"/>
       <c r="B66" s="17" t="s">
         <v>53</v>
@@ -19190,7 +19190,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="200"/>
       <c r="B67" s="17" t="s">
         <v>54</v>
@@ -19232,7 +19232,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="200" t="s">
         <v>190</v>
       </c>
@@ -19276,7 +19276,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="200"/>
       <c r="B69" s="17" t="s">
         <v>53</v>
@@ -19318,7 +19318,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="200"/>
       <c r="B70" s="17" t="s">
         <v>54</v>
@@ -19360,7 +19360,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="200" t="s">
         <v>191</v>
       </c>
@@ -19404,7 +19404,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="200"/>
       <c r="B72" s="17" t="s">
         <v>53</v>
@@ -19446,7 +19446,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="200"/>
       <c r="B73" s="17" t="s">
         <v>54</v>
@@ -19488,7 +19488,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="200" t="s">
         <v>192</v>
       </c>
@@ -19532,7 +19532,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="200"/>
       <c r="B75" s="17" t="s">
         <v>53</v>
@@ -19574,7 +19574,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="200"/>
       <c r="B76" s="17" t="s">
         <v>54</v>
@@ -19616,7 +19616,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="200" t="s">
         <v>193</v>
       </c>
@@ -19624,127 +19624,127 @@
         <v>51</v>
       </c>
       <c r="C77" s="19">
-        <v>0.5</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="D77" s="19">
-        <v>0.5</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="E77" s="19">
-        <v>0.5</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="F77" s="19">
-        <v>0.5</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="G77" s="19">
-        <v>0.5</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="H77" s="19">
-        <v>0.5</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="I77" s="19">
-        <v>0.5</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="J77" s="19">
-        <v>0.5</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="K77" s="19">
-        <v>0.5</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="L77" s="19">
-        <v>0.5</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="M77" s="19">
-        <v>0.5</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="N77" s="19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0.51900000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="200"/>
       <c r="B78" s="17" t="s">
         <v>53</v>
       </c>
       <c r="C78" s="19">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="D78" s="19">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="E78" s="19">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="F78" s="19">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="G78" s="19">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="H78" s="19">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="I78" s="19">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="J78" s="19">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="K78" s="19">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="L78" s="19">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="M78" s="19">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="N78" s="19">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="200"/>
       <c r="B79" s="17" t="s">
         <v>54</v>
       </c>
       <c r="C79" s="19">
-        <v>0.2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="D79" s="19">
-        <v>0.2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="E79" s="19">
-        <v>0.2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F79" s="19">
-        <v>0.2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="G79" s="19">
-        <v>0.2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="H79" s="19">
-        <v>0.2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="I79" s="19">
-        <v>0.2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="J79" s="19">
-        <v>0.2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="K79" s="19">
-        <v>0.2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="L79" s="19">
-        <v>0.2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="M79" s="19">
-        <v>0.2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="N79" s="19">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="200" t="s">
         <v>194</v>
       </c>
@@ -19752,127 +19752,139 @@
         <v>51</v>
       </c>
       <c r="C80" s="19">
-        <v>0.5</v>
+        <f t="shared" ref="C80:N80" si="0">1-C81-C82</f>
+        <v>0.13700000000000001</v>
       </c>
       <c r="D80" s="19">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="E80" s="19">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="F80" s="19">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="G80" s="19">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="H80" s="19">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="I80" s="19">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="J80" s="19">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="K80" s="19">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="L80" s="19">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="M80" s="19">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="N80" s="19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="200"/>
       <c r="B81" s="17" t="s">
         <v>53</v>
       </c>
       <c r="C81" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="D81" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="E81" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="F81" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="G81" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="H81" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="I81" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="J81" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="K81" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="L81" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="M81" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="N81" s="19">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0.85899999999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="200"/>
       <c r="B82" s="17" t="s">
         <v>54</v>
       </c>
       <c r="C82" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D82" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E82" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F82" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="G82" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H82" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="I82" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J82" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="K82" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="L82" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="M82" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="N82" s="19">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="200" t="s">
         <v>195</v>
       </c>
@@ -19880,127 +19892,139 @@
         <v>51</v>
       </c>
       <c r="C83" s="19">
-        <v>0.5</v>
+        <f t="shared" ref="C83:N83" si="1">1-C84-C85</f>
+        <v>0.13700000000000001</v>
       </c>
       <c r="D83" s="19">
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="E83" s="19">
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="F83" s="19">
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="G83" s="19">
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="H83" s="19">
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="I83" s="19">
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="J83" s="19">
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="K83" s="19">
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="L83" s="19">
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="M83" s="19">
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="N83" s="19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="200"/>
       <c r="B84" s="17" t="s">
         <v>53</v>
       </c>
       <c r="C84" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="D84" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="E84" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="F84" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="G84" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="H84" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="I84" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="J84" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="K84" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="L84" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="M84" s="19">
-        <v>0.2</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="N84" s="19">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0.85899999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="200"/>
       <c r="B85" s="17" t="s">
         <v>54</v>
       </c>
       <c r="C85" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D85" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E85" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F85" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="G85" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H85" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="I85" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J85" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="K85" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="L85" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="M85" s="19">
-        <v>0.2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="N85" s="19">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="200" t="s">
         <v>196</v>
       </c>
@@ -20044,7 +20068,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="200"/>
       <c r="B87" s="17" t="s">
         <v>53</v>
@@ -20086,7 +20110,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="200"/>
       <c r="B88" s="17" t="s">
         <v>54</v>
@@ -20128,7 +20152,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="200" t="s">
         <v>197</v>
       </c>
@@ -20172,7 +20196,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="200"/>
       <c r="B90" s="17" t="s">
         <v>53</v>
@@ -20214,7 +20238,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="200"/>
       <c r="B91" s="17" t="s">
         <v>54</v>
@@ -20256,7 +20280,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="200" t="s">
         <v>198</v>
       </c>
@@ -20300,7 +20324,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="200"/>
       <c r="B93" s="17" t="s">
         <v>53</v>
@@ -20342,7 +20366,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="200"/>
       <c r="B94" s="17" t="s">
         <v>54</v>
@@ -20384,7 +20408,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="200" t="s">
         <v>199</v>
       </c>
@@ -20428,7 +20452,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="200"/>
       <c r="B96" s="17" t="s">
         <v>53</v>
@@ -20470,7 +20494,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="200"/>
       <c r="B97" s="17" t="s">
         <v>54</v>
@@ -20512,7 +20536,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="200" t="s">
         <v>200</v>
       </c>
@@ -20556,7 +20580,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="200"/>
       <c r="B99" s="17" t="s">
         <v>53</v>
@@ -20598,7 +20622,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="200"/>
       <c r="B100" s="17" t="s">
         <v>54</v>
@@ -20640,7 +20664,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="200" t="s">
         <v>201</v>
       </c>
@@ -20684,7 +20708,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="200"/>
       <c r="B102" s="17" t="s">
         <v>53</v>
@@ -20726,7 +20750,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="200"/>
       <c r="B103" s="17" t="s">
         <v>54</v>
@@ -20768,7 +20792,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="200" t="s">
         <v>202</v>
       </c>
@@ -20812,7 +20836,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="200"/>
       <c r="B105" s="17" t="s">
         <v>53</v>
@@ -20854,7 +20878,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="200"/>
       <c r="B106" s="17" t="s">
         <v>54</v>
@@ -20896,7 +20920,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="200" t="s">
         <v>203</v>
       </c>
@@ -20940,7 +20964,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="200"/>
       <c r="B108" s="17" t="s">
         <v>53</v>
@@ -20982,7 +21006,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="200"/>
       <c r="B109" s="17" t="s">
         <v>54</v>
@@ -21024,7 +21048,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="177" t="s">
         <v>204</v>
       </c>
@@ -21068,7 +21092,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="198" t="s">
         <v>205</v>
       </c>
@@ -21112,7 +21136,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="198"/>
       <c r="B112" s="17" t="s">
         <v>207</v>
@@ -21154,7 +21178,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="116" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A116" s="197" t="s">
         <v>208</v>
       </c>
@@ -21188,7 +21212,7 @@
       <c r="AC116" s="197"/>
       <c r="AD116" s="197"/>
     </row>
-    <row r="117" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A117" s="17" t="s">
         <v>209</v>
       </c>
@@ -21280,7 +21304,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="118" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A118" s="17" t="s">
         <v>210</v>
       </c>

</xml_diff>